<commit_message>
Update Excel test suite to include more functions
- Pull dist values into separate xlsx file
</commit_message>
<xml_diff>
--- a/reeevr/test/excelunit/adaptive-tests.xlsx
+++ b/reeevr/test/excelunit/adaptive-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo14776\PycharmProjects\Excel-R-compiler\reeevr\test\excelunit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A018DEBA-F708-4A70-864C-C836D52E4495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D1C6D8-45CC-4265-B700-2357020B9358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A2A2A88B-2501-4D0B-BDBB-D0B2F7897C51}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2A2A88B-2501-4D0B-BDBB-D0B2F7897C51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Functions</t>
   </si>
@@ -77,9 +77,6 @@
     <t>LOWER</t>
   </si>
   <si>
-    <t>Array Functions</t>
-  </si>
-  <si>
     <t>Inputs</t>
   </si>
   <si>
@@ -132,6 +129,12 @@
   </si>
   <si>
     <t>^^%%££</t>
+  </si>
+  <si>
+    <t>NORMSINV</t>
+  </si>
+  <si>
+    <t>_xlfn.NORM.S.INV</t>
   </si>
 </sst>
 </file>
@@ -526,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5F0746-BD36-4A24-A5B0-69E2A8919C9E}">
   <dimension ref="B2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T20" sqref="B19:T20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,13 +543,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
@@ -573,27 +576,27 @@
         <v>2.7182818284590451</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:N3" si="0">LN(C3)</f>
+        <f>LN(C3)</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f>LN(D3)</f>
         <v>1.3862943611198906</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f>LN(E3)</f>
         <v>0.91629073187415511</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
+        <f>LN(F3)</f>
         <v>-2.3025850929940455</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
+        <f>LN(G3)</f>
         <v>4.5849674786705723</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
+        <f>LN(H3)</f>
         <v>1</v>
       </c>
       <c r="O3">
@@ -902,7 +905,7 @@
         <v>1.1051709180756477</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:N8" si="1">_xlfn.LOGNORM.INV(0.5,D8,E8)</f>
+        <f>_xlfn.LOGNORM.INV(0.5,D8,E8)</f>
         <v>7.3890560989306504</v>
       </c>
       <c r="K8">
@@ -914,11 +917,11 @@
         <v>4.9787068367863944E-2</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f>_xlfn.LOGNORM.INV(0.5,G8,H8)</f>
         <v>7.3890560989306504</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f>_xlfn.LOGNORM.INV(0.5,H8,I8)</f>
         <v>2.7182818284590451</v>
       </c>
       <c r="O8">
@@ -942,7 +945,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -1032,23 +1035,23 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10:N10" si="2">INT(D10)</f>
+        <f>INT(D10)</f>
         <v>-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f>INT(E10)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f>INT(F10)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
+        <f>INT(G10)</f>
         <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f>INT(H10)</f>
         <v>-2</v>
       </c>
       <c r="O10">
@@ -1075,41 +1078,41 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
       </c>
       <c r="F11">
         <v>123</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" t="str">
         <f>UPPER(C11)</f>
         <v>ASDASF</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:M11" si="3">UPPER(D11)</f>
+        <f>UPPER(D11)</f>
         <v>ASDASF</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="3"/>
+        <f>UPPER(E11)</f>
         <v>ASDASF</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="3"/>
+        <f>UPPER(F11)</f>
         <v>123</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="3"/>
+        <f>UPPER(G11)</f>
         <v>A12SD!</v>
       </c>
       <c r="N11" t="str">
@@ -1117,22 +1120,22 @@
         <v>A1265A!</v>
       </c>
       <c r="O11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S11" t="s">
         <v>20</v>
       </c>
-      <c r="P11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" t="s">
-        <v>22</v>
-      </c>
-      <c r="S11" t="s">
-        <v>21</v>
-      </c>
       <c r="T11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -1140,64 +1143,64 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
       </c>
       <c r="F12">
         <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" t="str">
         <f>LOWER(C12)</f>
         <v>asdasf</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:N12" si="4">LOWER(D12)</f>
+        <f>LOWER(D12)</f>
         <v>asdasf</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="4"/>
+        <f>LOWER(E12)</f>
         <v>asdasf</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="4"/>
+        <f>LOWER(F12)</f>
         <v>124</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="4"/>
+        <f>LOWER(G12)</f>
         <v>a12sd!</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="4"/>
+        <f>LOWER(H12)</f>
         <v>a1265a!</v>
       </c>
       <c r="O12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R12" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" t="s">
         <v>23</v>
       </c>
-      <c r="S12" t="s">
-        <v>24</v>
-      </c>
       <c r="T12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -1214,36 +1217,36 @@
         <v>21</v>
       </c>
       <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13">
         <f>LEN(C13)</f>
         <v>3</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:N13" si="5">LEN(D13)</f>
+        <f>LEN(D13)</f>
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="5"/>
+        <f>LEN(E13)</f>
         <v>2</v>
       </c>
       <c r="L13">
-        <f t="shared" si="5"/>
+        <f>LEN(F13)</f>
         <v>4</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f>LEN(G13)</f>
         <v>5</v>
       </c>
       <c r="N13">
-        <f t="shared" si="5"/>
+        <f>LEN(H13)</f>
         <v>6</v>
       </c>
       <c r="O13">
@@ -1265,148 +1268,269 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>2.5</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.STDEV.S(C14:H14)</f>
+        <v>14.409776773658455</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:N14" si="0">_xlfn.STDEV.S(D14:I14)</f>
+        <v>13.481021807080554</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>12.255524515131569</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>10.860781640873398</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>8.9863361938997581</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>7.5958551555650491</v>
+      </c>
+      <c r="O14">
+        <v>14.409776773658455</v>
+      </c>
+      <c r="P14">
+        <v>13.481021807080554</v>
+      </c>
+      <c r="Q14">
+        <v>12.255524515131569</v>
+      </c>
+      <c r="R14">
+        <v>10.860781640873398</v>
+      </c>
+      <c r="S14">
+        <v>8.9863361938997581</v>
+      </c>
+      <c r="T14">
+        <v>7.5958551555650491</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <f>STDEV(C15:H15)</f>
+        <v>14.409776773658455</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:N15" si="1">STDEV(D15:I15)</f>
+        <v>13.481021807080554</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>12.255524515131569</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>10.860781640873398</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>8.9863361938997581</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>7.5958551555650491</v>
+      </c>
+      <c r="O15">
+        <v>14.409776773658455</v>
+      </c>
+      <c r="P15">
+        <v>13.481021807080554</v>
+      </c>
+      <c r="Q15">
+        <v>12.255524515131569</v>
+      </c>
+      <c r="R15">
+        <v>10.860781640873398</v>
+      </c>
+      <c r="S15">
+        <v>8.9863361938997581</v>
+      </c>
+      <c r="T15">
+        <v>7.5958551555650491</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C16">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F16">
-        <v>2.5</v>
+        <v>0.6</v>
       </c>
       <c r="G16">
-        <v>30</v>
+        <v>0.9</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>0.65</v>
       </c>
       <c r="I16">
-        <f>AVERAGE(C16:H16)</f>
-        <v>11.416666666666666</v>
+        <f>NORMSINV(C16)</f>
+        <v>-0.84162123357291452</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:N16" si="6">AVERAGE(D16:I16)</f>
-        <v>13.152777777777779</v>
+        <f t="shared" ref="J16:N16" si="2">NORMSINV(D16)</f>
+        <v>-1.2815515655446006</v>
       </c>
       <c r="K16">
-        <f t="shared" si="6"/>
-        <v>15.011574074074076</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="L16">
-        <f t="shared" si="6"/>
-        <v>17.013503086419757</v>
+        <f t="shared" si="2"/>
+        <v>0.25334710313579978</v>
       </c>
       <c r="M16">
-        <f t="shared" si="6"/>
-        <v>19.432420267489714</v>
+        <f t="shared" si="2"/>
+        <v>1.2815515655446006</v>
       </c>
       <c r="N16">
-        <f t="shared" si="6"/>
-        <v>17.671156978738001</v>
+        <f t="shared" si="2"/>
+        <v>0.38532046640756784</v>
       </c>
       <c r="O16">
-        <v>11.416666666666666</v>
+        <v>-0.84162123357291452</v>
       </c>
       <c r="P16">
-        <v>13.152777777777779</v>
+        <v>-1.2815515655446006</v>
       </c>
       <c r="Q16">
-        <v>15.011574074074076</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>17.013503086419757</v>
+        <v>0.25334710313579978</v>
       </c>
       <c r="S16">
-        <v>19.432420267489714</v>
+        <v>1.2815515655446006</v>
       </c>
       <c r="T16">
-        <v>17.671156978738001</v>
+        <v>0.38532046640756784</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>0.6</v>
+      </c>
+      <c r="G17">
+        <v>0.9</v>
+      </c>
+      <c r="H17">
+        <v>0.65</v>
+      </c>
+      <c r="I17">
+        <f>_xlfn.NORM.S.INV(C17)</f>
+        <v>-0.84162123357291452</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:N17" si="3">_xlfn.NORM.S.INV(D17)</f>
+        <v>-1.2815515655446006</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>0.25334710313579978</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>1.2815515655446006</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>0.38532046640756784</v>
+      </c>
+      <c r="O17">
+        <v>-0.84162123357291452</v>
+      </c>
+      <c r="P17">
+        <v>-1.2815515655446006</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0.25334710313579978</v>
+      </c>
+      <c r="S17">
+        <v>1.2815515655446006</v>
+      </c>
+      <c r="T17">
+        <v>0.38532046640756784</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <v>2.5</v>
-      </c>
-      <c r="G17">
-        <v>30</v>
-      </c>
-      <c r="H17">
-        <v>30</v>
-      </c>
-      <c r="I17">
-        <f>_xlfn.STDEV.S(C17:H17)</f>
-        <v>14.409776773658455</v>
-      </c>
-      <c r="J17">
-        <f t="shared" ref="J17:N17" si="7">_xlfn.STDEV.S(D17:I17)</f>
-        <v>13.481021807080554</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="7"/>
-        <v>12.255524515131569</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="7"/>
-        <v>10.860781640873398</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="7"/>
-        <v>8.9863361938997581</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="7"/>
-        <v>7.5958551555650491</v>
-      </c>
-      <c r="O17">
-        <v>14.409776773658455</v>
-      </c>
-      <c r="P17">
-        <v>13.481021807080554</v>
-      </c>
-      <c r="Q17">
-        <v>12.255524515131569</v>
-      </c>
-      <c r="R17">
-        <v>10.860781640873398</v>
-      </c>
-      <c r="S17">
-        <v>8.9863361938997581</v>
-      </c>
-      <c r="T17">
-        <v>7.5958551555650491</v>
-      </c>
-    </row>
-    <row r="18" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1418,59 +1542,121 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>2.5</v>
+        <v>-4</v>
       </c>
       <c r="G18">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I18">
-        <f>STDEV(C18:H18)</f>
-        <v>14.409776773658455</v>
+        <f>AVERAGE(C18:H18)</f>
+        <v>2.1666666666666665</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:N18" si="8">STDEV(D18:I18)</f>
-        <v>13.481021807080554</v>
+        <f t="shared" ref="J18:N18" si="4">AVERAGE(D18:I18)</f>
+        <v>2.3611111111111112</v>
       </c>
       <c r="K18">
-        <f t="shared" si="8"/>
-        <v>12.255524515131569</v>
+        <f t="shared" si="4"/>
+        <v>2.4212962962962963</v>
       </c>
       <c r="L18">
-        <f t="shared" si="8"/>
-        <v>10.860781640873398</v>
+        <f t="shared" si="4"/>
+        <v>2.3248456790123453</v>
       </c>
       <c r="M18">
-        <f t="shared" si="8"/>
-        <v>8.9863361938997581</v>
+        <f t="shared" si="4"/>
+        <v>3.3789866255144028</v>
       </c>
       <c r="N18">
-        <f t="shared" si="8"/>
-        <v>7.5958551555650491</v>
+        <f t="shared" si="4"/>
+        <v>3.1088177297668036</v>
       </c>
       <c r="O18">
-        <v>14.409776773658455</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="P18">
-        <v>13.481021807080554</v>
+        <v>2.3611111111111112</v>
       </c>
       <c r="Q18">
-        <v>12.255524515131569</v>
+        <v>2.4212962962962963</v>
       </c>
       <c r="R18">
-        <v>10.860781640873398</v>
+        <v>2.3248456790123453</v>
       </c>
       <c r="S18">
-        <v>8.9863361938997581</v>
+        <v>3.3789866255144028</v>
       </c>
       <c r="T18">
-        <v>7.5958551555650491</v>
+        <v>3.1088177297668036</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>-4</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <f>AVERAGE(C19,D19,E19,F19,G19,H19)</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ref="J19:N19" si="5">AVERAGE(D19,E19,F19,G19,H19,I19)</f>
+        <v>2.3611111111111112</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>2.4212962962962963</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>2.3248456790123453</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>3.3789866255144028</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>3.1088177297668036</v>
+      </c>
+      <c r="O19">
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="P19">
+        <v>2.3611111111111112</v>
+      </c>
+      <c r="Q19">
+        <v>2.4212962962962963</v>
+      </c>
+      <c r="R19">
+        <v>2.3248456790123453</v>
+      </c>
+      <c r="S19">
+        <v>3.3789866255144028</v>
+      </c>
+      <c r="T19">
+        <v>3.1088177297668036</v>
+      </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -1480,5 +1666,6 @@
     <hyperlink ref="G13" r:id="rId1" xr:uid="{195215D6-96AC-4D8E-AAF1-BDB0309BA3A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>